<commit_message>
blockchain comparison sheet add edit
</commit_message>
<xml_diff>
--- a/INTRblockchainOptionCompare.xlsx
+++ b/INTRblockchainOptionCompare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/blairmunroakusa/DUMP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{644DA7C8-DA37-F447-82BC-02F2E42B411A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{064B9E20-A754-F943-B4D0-B05E1FE0A7EF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="660" yWindow="500" windowWidth="37740" windowHeight="23500" xr2:uid="{DFD451E1-097A-ED4F-8BEB-59B22B685EBA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="66">
   <si>
     <t>substrate core</t>
   </si>
@@ -99,18 +99,6 @@
     <t>tx total</t>
   </si>
   <si>
-    <t>75b</t>
-  </si>
-  <si>
-    <t>7m</t>
-  </si>
-  <si>
-    <t>15m</t>
-  </si>
-  <si>
-    <t>11m</t>
-  </si>
-  <si>
     <t>contracts</t>
   </si>
   <si>
@@ -238,6 +226,12 @@
   </si>
   <si>
     <t>640,000</t>
+  </si>
+  <si>
+    <t>75,000,000,000</t>
+  </si>
+  <si>
+    <t>7,000,000</t>
   </si>
 </sst>
 </file>
@@ -352,7 +346,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -394,6 +388,8 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -711,7 +707,7 @@
   <dimension ref="B4:L26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="M36" sqref="M36"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -781,24 +777,24 @@
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="18" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="19" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="H8" s="20" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="I8" s="6"/>
       <c r="J8" s="19" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="K8" s="20" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.2">
@@ -807,24 +803,24 @@
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="18" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="19" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="H9" s="20" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="I9" s="6"/>
       <c r="J9" s="19" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="K9" s="20" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.2">
@@ -910,8 +906,8 @@
         <v>20</v>
       </c>
       <c r="C13" s="3"/>
-      <c r="D13" s="5" t="s">
-        <v>21</v>
+      <c r="D13" s="18" t="s">
+        <v>64</v>
       </c>
       <c r="E13" t="s">
         <v>13</v>
@@ -919,14 +915,14 @@
       <c r="G13" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="H13" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="J13" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="K13" s="13" t="s">
-        <v>24</v>
+      <c r="H13" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="J13" s="21">
+        <v>15000000</v>
+      </c>
+      <c r="K13" s="22">
+        <v>11000000</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.2">
@@ -939,82 +935,82 @@
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B15" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E15" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="H15" s="13" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="J15" s="12" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="K15" s="13" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B16" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E16" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="J16" s="12" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="K16" s="13" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B17" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E17" t="s">
         <v>13</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H17" s="13" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="J17" s="12" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="K17" s="13" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B18" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E18" t="s">
         <v>13</v>
@@ -1034,22 +1030,22 @@
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B19" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E19" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H19" s="13" t="s">
         <v>13</v>
       </c>
       <c r="J19" s="12" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="K19" s="13" t="s">
         <v>13</v>
@@ -1057,125 +1053,125 @@
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B20" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D20" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20" t="s">
+        <v>34</v>
+      </c>
+      <c r="G20" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E20" t="s">
+      <c r="H20" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="J20" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="G20" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="H20" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="J20" s="12" t="s">
-        <v>42</v>
-      </c>
       <c r="K20" s="13" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B21" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E21" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G21" s="12" t="s">
         <v>11</v>
       </c>
       <c r="H21" s="13" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="J21" s="12" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="K21" s="13" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B22" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E22" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G22" s="12" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H22" s="13" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="J22" s="12" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="K22" s="13" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="L22" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B23" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E23" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H23" s="13" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="J23" s="12" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="K23" s="13" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E24" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G24" s="16" t="s">
         <v>11</v>
       </c>
       <c r="H24" s="17" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="J24" s="16" t="s">
         <v>11</v>
       </c>
       <c r="K24" s="17" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B26" s="7" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1185,7 +1181,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="D11:D12 H10 D18 D8:K9" numberStoredAsText="1"/>
+    <ignoredError sqref="D11:D13 H10 D18 D8:K9 H13" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>